<commit_message>
Updated compiled data spreadsheet
</commit_message>
<xml_diff>
--- a/CompiledData.xlsx
+++ b/CompiledData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maitreyi\Documents\MIT\Courses\Spring22\6.882\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA21468-E738-4BFE-8F99-A7E823C83F82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05526A6-7BBC-4F4B-9F5A-EEAC7031A07C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5268" xr2:uid="{3D0962EF-CBB4-4902-9933-AFB3BC885659}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5268" activeTab="4" xr2:uid="{3D0962EF-CBB4-4902-9933-AFB3BC885659}"/>
   </bookViews>
   <sheets>
     <sheet name="Circuits_Papers" sheetId="1" r:id="rId1"/>
@@ -6169,7 +6169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69DBFA5-4FAA-4640-A5A4-F7F2DD305A9F}">
   <dimension ref="A1:Q250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="L239" sqref="L239"/>
     </sheetView>
   </sheetViews>
@@ -24070,7 +24070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E3D87D-B947-44BA-A0D5-696BBA9F1397}">
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView topLeftCell="C52" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="C64" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
@@ -25805,8 +25805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDF9583-2435-4BFD-858E-D7515FDF4D6D}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>